<commit_message>
feat: update export billing detail Excel file
</commit_message>
<xml_diff>
--- a/resources/xlsx/export_billing_detail.xlsx
+++ b/resources/xlsx/export_billing_detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mmj\project\PHP\MARGO-BARU\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FC2B05-353F-42FE-B2D1-20809C478DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F589E400-8D22-4A3A-9172-55336CD90A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{16F53B30-EA35-46C9-9529-5DBEDB6DC1E5}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>Saldo Hutang</t>
   </si>
   <si>
-    <t>SALDO BILLING [semester]</t>
-  </si>
-  <si>
     <t>[salesperson.marketing_area.name]</t>
   </si>
   <si>
@@ -582,6 +579,9 @@
   </si>
   <si>
     <t>[current_bills]</t>
+  </si>
+  <si>
+    <t>SALDO BILLING [semester] - [salesperson.name]</t>
   </si>
 </sst>
 </file>
@@ -862,6 +862,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -906,9 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -932,12 +932,6 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -965,8 +959,14 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1308,7 +1308,7 @@
   <dimension ref="A2:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:J4"/>
+      <selection activeCell="C5" sqref="C5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,66 +1321,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D6" s="7"/>
@@ -1392,29 +1392,29 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="G8" s="51" t="s">
-        <v>170</v>
+      <c r="E8" s="28"/>
+      <c r="G8" s="49" t="s">
+        <v>169</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I8" s="58"/>
     </row>
@@ -1422,54 +1422,54 @@
       <c r="A9" s="5">
         <v>1</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="56"/>
       <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+      <c r="F10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="45">
-        <v>0</v>
-      </c>
-      <c r="E11" s="46"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="43">
+        <v>0</v>
+      </c>
+      <c r="E11" s="44"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -1478,12 +1478,12 @@
       <c r="I14" s="14"/>
       <c r="J14" s="16"/>
       <c r="K14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>6</v>
@@ -1513,7 +1513,7 @@
         <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1521,78 +1521,78 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="G16" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="H16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="J16" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="35" t="s">
-        <v>35</v>
-      </c>
       <c r="K16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="8">
         <f>SUM(G16:G16)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="47">
+      <c r="H17" s="45">
         <f>SUM(H16:H16)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="45">
         <f>SUM(I16:I16)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="48">
+      <c r="J17" s="46">
         <f>SUM(J16:J16)</f>
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -1601,12 +1601,12 @@
       <c r="I19" s="14"/>
       <c r="J19" s="16"/>
       <c r="K19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
@@ -1636,7 +1636,7 @@
         <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1644,63 +1644,63 @@
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="G21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="H21" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="I21" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="J21" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="35" t="s">
-        <v>46</v>
-      </c>
       <c r="K21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="8">
         <f>SUM(G21:G21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="47">
+      <c r="H22" s="45">
         <f>SUM(H21:H21)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="47">
+      <c r="I22" s="45">
         <f>SUM(I21:I21)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="48">
+      <c r="J22" s="46">
         <f>SUM(J21:J21)</f>
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1713,17 +1713,17 @@
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
       <c r="K23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1732,12 +1732,12 @@
       <c r="I24" s="14"/>
       <c r="J24" s="16"/>
       <c r="K24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
@@ -1767,7 +1767,7 @@
         <v>4</v>
       </c>
       <c r="K25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1775,63 +1775,63 @@
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="G26" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="H26" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="I26" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="J26" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="35" t="s">
-        <v>59</v>
-      </c>
       <c r="K26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="8">
         <f>SUM(G26:G26)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="47">
+      <c r="H27" s="45">
         <f>SUM(H26:H26)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="47">
+      <c r="I27" s="45">
         <f>SUM(I26:I26)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="48">
+      <c r="J27" s="46">
         <f>SUM(J26:J26)</f>
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1844,17 +1844,17 @@
       <c r="I28" s="11"/>
       <c r="J28" s="9"/>
       <c r="K28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -1863,12 +1863,12 @@
       <c r="I29" s="14"/>
       <c r="J29" s="16"/>
       <c r="K29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -1898,7 +1898,7 @@
         <v>4</v>
       </c>
       <c r="K30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1906,63 +1906,63 @@
         <v>1</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="G31" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="33" t="s">
+      <c r="H31" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="I31" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="J31" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="J31" s="35" t="s">
-        <v>71</v>
-      </c>
       <c r="K31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="8">
         <f>SUM(G31:G31)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="47">
+      <c r="H32" s="45">
         <f>SUM(H31:H31)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="47">
+      <c r="I32" s="45">
         <f>SUM(I31:I31)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="48">
+      <c r="J32" s="46">
         <f>SUM(J31:J31)</f>
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1975,17 +1975,17 @@
       <c r="I33" s="11"/>
       <c r="J33" s="9"/>
       <c r="K33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -1994,12 +1994,12 @@
       <c r="I34" s="14"/>
       <c r="J34" s="16"/>
       <c r="K34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>6</v>
@@ -2029,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="K35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2037,63 +2037,63 @@
         <v>1</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="G36" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="33" t="s">
+      <c r="H36" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="I36" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="J36" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="J36" s="35" t="s">
-        <v>84</v>
-      </c>
       <c r="K36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="8">
         <f>SUM(G36:G36)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="49">
+      <c r="H37" s="47">
         <f>SUM(H36:H36)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="49">
+      <c r="I37" s="47">
         <f>SUM(I36:I36)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="50">
+      <c r="J37" s="48">
         <f>SUM(J36:J36)</f>
         <v>0</v>
       </c>
       <c r="K37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -2106,17 +2106,17 @@
       <c r="I38" s="11"/>
       <c r="J38" s="9"/>
       <c r="K38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
       <c r="D39" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2125,12 +2125,12 @@
       <c r="I39" s="14"/>
       <c r="J39" s="16"/>
       <c r="K39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>6</v>
@@ -2160,7 +2160,7 @@
         <v>4</v>
       </c>
       <c r="K40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2168,63 +2168,63 @@
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="G41" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G41" s="33" t="s">
+      <c r="H41" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="I41" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="J41" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="J41" s="35" t="s">
-        <v>96</v>
-      </c>
       <c r="K41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
       <c r="G42" s="8">
         <f>SUM(G41:G41)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="49">
+      <c r="H42" s="47">
         <f>SUM(H41:H41)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="49">
+      <c r="I42" s="47">
         <f>SUM(I41:I41)</f>
         <v>0</v>
       </c>
-      <c r="J42" s="50">
+      <c r="J42" s="48">
         <f>SUM(J41:J41)</f>
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2237,17 +2237,17 @@
       <c r="I43" s="11"/>
       <c r="J43" s="9"/>
       <c r="K43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
       <c r="D44" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
@@ -2256,12 +2256,12 @@
       <c r="I44" s="14"/>
       <c r="J44" s="16"/>
       <c r="K44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>6</v>
@@ -2291,7 +2291,7 @@
         <v>4</v>
       </c>
       <c r="K45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2299,63 +2299,63 @@
         <v>1</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="F46" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="G46" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="33" t="s">
+      <c r="H46" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="I46" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="J46" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="J46" s="35" t="s">
-        <v>108</v>
-      </c>
       <c r="K46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
       <c r="G47" s="8">
         <f>SUM(G46:G46)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="49">
+      <c r="H47" s="47">
         <f>SUM(H46:H46)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="49">
+      <c r="I47" s="47">
         <f>SUM(I46:I46)</f>
         <v>0</v>
       </c>
-      <c r="J47" s="50">
+      <c r="J47" s="48">
         <f>SUM(J46:J46)</f>
         <v>0</v>
       </c>
       <c r="K47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -2368,17 +2368,17 @@
       <c r="I48" s="11"/>
       <c r="J48" s="9"/>
       <c r="K48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -2387,12 +2387,12 @@
       <c r="I49" s="14"/>
       <c r="J49" s="16"/>
       <c r="K49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>6</v>
@@ -2422,7 +2422,7 @@
         <v>4</v>
       </c>
       <c r="K50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -2430,63 +2430,63 @@
         <v>1</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="E51" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="F51" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="F51" s="34" t="s">
+      <c r="G51" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="33" t="s">
+      <c r="H51" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="H51" s="17" t="s">
+      <c r="I51" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="I51" s="17" t="s">
+      <c r="J51" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="J51" s="35" t="s">
-        <v>120</v>
-      </c>
       <c r="K51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
       <c r="G52" s="8">
         <f>SUM(G51:G51)</f>
         <v>0</v>
       </c>
-      <c r="H52" s="49">
+      <c r="H52" s="47">
         <f>SUM(H51:H51)</f>
         <v>0</v>
       </c>
-      <c r="I52" s="49">
+      <c r="I52" s="47">
         <f>SUM(I51:I51)</f>
         <v>0</v>
       </c>
-      <c r="J52" s="50">
+      <c r="J52" s="48">
         <f>SUM(J51:J51)</f>
         <v>0</v>
       </c>
       <c r="K52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -2499,17 +2499,17 @@
       <c r="I53" s="11"/>
       <c r="J53" s="9"/>
       <c r="K53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -2518,12 +2518,12 @@
       <c r="I54" s="14"/>
       <c r="J54" s="16"/>
       <c r="K54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>6</v>
@@ -2553,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="K55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -2561,63 +2561,63 @@
         <v>1</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="E56" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="F56" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="F56" s="34" t="s">
+      <c r="G56" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="G56" s="33" t="s">
+      <c r="H56" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="H56" s="17" t="s">
+      <c r="I56" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="I56" s="17" t="s">
+      <c r="J56" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="J56" s="35" t="s">
-        <v>132</v>
-      </c>
       <c r="K56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
       <c r="G57" s="8">
         <f>SUM(G56:G56)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="49">
+      <c r="H57" s="47">
         <f>SUM(H56:H56)</f>
         <v>0</v>
       </c>
-      <c r="I57" s="49">
+      <c r="I57" s="47">
         <f>SUM(I56:I56)</f>
         <v>0</v>
       </c>
-      <c r="J57" s="50">
+      <c r="J57" s="48">
         <f>SUM(J56:J56)</f>
         <v>0</v>
       </c>
       <c r="K57" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -2630,17 +2630,17 @@
       <c r="I58" s="11"/>
       <c r="J58" s="9"/>
       <c r="K58" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
       <c r="D59" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2649,12 +2649,12 @@
       <c r="I59" s="14"/>
       <c r="J59" s="16"/>
       <c r="K59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>6</v>
@@ -2684,7 +2684,7 @@
         <v>4</v>
       </c>
       <c r="K60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -2692,63 +2692,63 @@
         <v>1</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="D61" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="E61" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="F61" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="F61" s="34" t="s">
+      <c r="G61" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="G61" s="33" t="s">
+      <c r="H61" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="H61" s="17" t="s">
+      <c r="I61" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="J61" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="J61" s="35" t="s">
-        <v>144</v>
-      </c>
       <c r="K61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
       <c r="G62" s="8">
         <f>SUM(G61:G61)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="49">
+      <c r="H62" s="47">
         <f>SUM(H61:H61)</f>
         <v>0</v>
       </c>
-      <c r="I62" s="49">
+      <c r="I62" s="47">
         <f>SUM(I61:I61)</f>
         <v>0</v>
       </c>
-      <c r="J62" s="50">
+      <c r="J62" s="48">
         <f>SUM(J61:J61)</f>
         <v>0</v>
       </c>
       <c r="K62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -2761,17 +2761,17 @@
       <c r="I63" s="11"/>
       <c r="J63" s="9"/>
       <c r="K63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
@@ -2780,12 +2780,12 @@
       <c r="I64" s="14"/>
       <c r="J64" s="16"/>
       <c r="K64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>6</v>
@@ -2815,7 +2815,7 @@
         <v>4</v>
       </c>
       <c r="K65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -2823,63 +2823,63 @@
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="D66" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="E66" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="F66" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="F66" s="34" t="s">
+      <c r="G66" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G66" s="33" t="s">
+      <c r="H66" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="H66" s="17" t="s">
+      <c r="I66" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="I66" s="17" t="s">
+      <c r="J66" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="J66" s="35" t="s">
-        <v>156</v>
-      </c>
       <c r="K66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
       <c r="G67" s="8">
         <f>SUM(G66:G66)</f>
         <v>0</v>
       </c>
-      <c r="H67" s="49">
+      <c r="H67" s="47">
         <f>SUM(H66:H66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="49">
+      <c r="I67" s="47">
         <f>SUM(I66:I66)</f>
         <v>0</v>
       </c>
-      <c r="J67" s="50">
+      <c r="J67" s="48">
         <f>SUM(J66:J66)</f>
         <v>0</v>
       </c>
       <c r="K67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -2892,22 +2892,22 @@
       <c r="I68" s="11"/>
       <c r="J68" s="9"/>
       <c r="K68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
       <c r="D69" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="16"/>
       <c r="G69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
@@ -2915,12 +2915,12 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B70" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="25"/>
+        <v>157</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" s="26"/>
       <c r="D70" s="3" t="s">
         <v>10</v>
       </c>
@@ -2928,34 +2928,34 @@
         <v>11</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="9"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="53">
+      <c r="A71" s="51">
         <v>1</v>
       </c>
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="C71" s="52"/>
+      <c r="D71" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="E71" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="F71" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="G71" t="s">
         <v>178</v>
-      </c>
-      <c r="C71" s="54"/>
-      <c r="D71" s="55" t="s">
-        <v>176</v>
-      </c>
-      <c r="E71" s="55" t="s">
-        <v>177</v>
-      </c>
-      <c r="F71" s="56" t="s">
-        <v>180</v>
-      </c>
-      <c r="G71" t="s">
-        <v>179</v>
       </c>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
@@ -2967,7 +2967,7 @@
       <c r="E72" s="9"/>
       <c r="F72" s="11"/>
       <c r="G72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
@@ -2975,31 +2975,31 @@
     </row>
     <row r="73" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B74" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="C74" s="25"/>
+      <c r="C74" s="26"/>
       <c r="D74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E74" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
@@ -3007,45 +3007,45 @@
         <v>1</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="F75" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="E75" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="F75" s="39" t="s">
-        <v>164</v>
-      </c>
       <c r="G75" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H75" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="I75" s="50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="I75" s="52" t="s">
+      <c r="B76" s="31"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="50" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
-      <c r="G76" s="30"/>
-      <c r="H76" s="31"/>
-      <c r="I76" s="52" t="s">
-        <v>172</v>
-      </c>
-    </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B77" s="36"/>

</xml_diff>

<commit_message>
feat: include return_good data
</commit_message>
<xml_diff>
--- a/resources/xlsx/export_billing_detail.xlsx
+++ b/resources/xlsx/export_billing_detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mmj\project\PHP\MARGO-BARU\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E2F98F-9425-44F1-9894-01B23DCDE12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47E5262-6FE1-4C35-8304-D5A59D28E51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{16F53B30-EA35-46C9-9529-5DBEDB6DC1E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="439">
   <si>
     <t>Nama Sales</t>
   </si>
@@ -575,9 +575,6 @@
     <t>[current_bills]</t>
   </si>
   <si>
-    <t>SALDO BILLING [semester] - [salesperson.name]</t>
-  </si>
-  <si>
     <t>FAKTUR PEMBAYARAN</t>
   </si>
   <si>
@@ -1179,6 +1176,183 @@
   </si>
   <si>
     <t>[additional_invoices5.nominal]</t>
+  </si>
+  <si>
+    <t>SALDO BILLING [semester] - [salesperson.name] - [salesperson.marketing_area.name]</t>
+  </si>
+  <si>
+    <t>FAKTUR RETUR</t>
+  </si>
+  <si>
+    <t>[returs1.number]</t>
+  </si>
+  <si>
+    <t>[returs1.date]</t>
+  </si>
+  <si>
+    <t>[=returs1]</t>
+  </si>
+  <si>
+    <t>[returs1.items.jenjang]</t>
+  </si>
+  <si>
+    <t>[returs1.items.mapel]</t>
+  </si>
+  <si>
+    <t>[returs1.items.kelas]</t>
+  </si>
+  <si>
+    <t>[returs1.items.halaman]</t>
+  </si>
+  <si>
+    <t>[returs1.items.price]</t>
+  </si>
+  <si>
+    <t>[returs1.items.quantity]</t>
+  </si>
+  <si>
+    <t>[returs1.items.total]</t>
+  </si>
+  <si>
+    <t>[returs1.items.subtotal]</t>
+  </si>
+  <si>
+    <t>[!returs1]</t>
+  </si>
+  <si>
+    <t>[returs2.number]</t>
+  </si>
+  <si>
+    <t>[returs2.date]</t>
+  </si>
+  <si>
+    <t>[=returs2]</t>
+  </si>
+  <si>
+    <t>[returs2.items.jenjang]</t>
+  </si>
+  <si>
+    <t>[returs2.items.mapel]</t>
+  </si>
+  <si>
+    <t>[returs2.items.kelas]</t>
+  </si>
+  <si>
+    <t>[returs2.items.halaman]</t>
+  </si>
+  <si>
+    <t>[returs2.items.price]</t>
+  </si>
+  <si>
+    <t>[returs2.items.quantity]</t>
+  </si>
+  <si>
+    <t>[returs2.items.total]</t>
+  </si>
+  <si>
+    <t>[returs2.items.subtotal]</t>
+  </si>
+  <si>
+    <t>[returs3.number]</t>
+  </si>
+  <si>
+    <t>[returs3.date]</t>
+  </si>
+  <si>
+    <t>[=returs3]</t>
+  </si>
+  <si>
+    <t>[returs3.items.jenjang]</t>
+  </si>
+  <si>
+    <t>[returs3.items.mapel]</t>
+  </si>
+  <si>
+    <t>[returs3.items.kelas]</t>
+  </si>
+  <si>
+    <t>[returs3.items.halaman]</t>
+  </si>
+  <si>
+    <t>[returs3.items.price]</t>
+  </si>
+  <si>
+    <t>[returs3.items.quantity]</t>
+  </si>
+  <si>
+    <t>[returs3.items.total]</t>
+  </si>
+  <si>
+    <t>[returs3.items.subtotal]</t>
+  </si>
+  <si>
+    <t>[returs4.number]</t>
+  </si>
+  <si>
+    <t>[returs4.date]</t>
+  </si>
+  <si>
+    <t>[=returs4]</t>
+  </si>
+  <si>
+    <t>[returs4.items.jenjang]</t>
+  </si>
+  <si>
+    <t>[returs4.items.mapel]</t>
+  </si>
+  <si>
+    <t>[returs4.items.kelas]</t>
+  </si>
+  <si>
+    <t>[returs4.items.halaman]</t>
+  </si>
+  <si>
+    <t>[returs4.items.price]</t>
+  </si>
+  <si>
+    <t>[returs4.items.quantity]</t>
+  </si>
+  <si>
+    <t>[returs4.items.total]</t>
+  </si>
+  <si>
+    <t>[returs4.items.subtotal]</t>
+  </si>
+  <si>
+    <t>[returs5.number]</t>
+  </si>
+  <si>
+    <t>[returs5.date]</t>
+  </si>
+  <si>
+    <t>[=returs5]</t>
+  </si>
+  <si>
+    <t>[returs5.items.jenjang]</t>
+  </si>
+  <si>
+    <t>[returs5.items.mapel]</t>
+  </si>
+  <si>
+    <t>[returs5.items.kelas]</t>
+  </si>
+  <si>
+    <t>[returs5.items.halaman]</t>
+  </si>
+  <si>
+    <t>[returs5.items.price]</t>
+  </si>
+  <si>
+    <t>[returs5.items.quantity]</t>
+  </si>
+  <si>
+    <t>[returs5.items.total]</t>
+  </si>
+  <si>
+    <t>[returs5.items.subtotal]</t>
+  </si>
+  <si>
+    <t>Belum Ada Retur</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1362,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;Rp&quot;#,##0;[Red]\-&quot;Rp&quot;#,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1422,7 +1596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1456,20 +1630,88 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1480,88 +1722,16 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1902,10 +2072,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K168"/>
+  <dimension ref="A2:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" topLeftCell="B172" workbookViewId="0">
+      <selection activeCell="H164" sqref="H164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,66 +2088,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="A2" s="48" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="23" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D6" s="7"/>
@@ -1989,71 +2159,71 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="G8" s="47" t="s">
+      <c r="E8" s="41"/>
+      <c r="G8" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="I8" s="56"/>
+      <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="53" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="43"/>
       <c r="F9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
       <c r="F10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="57">
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46">
         <f>SUM(D9:D9)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="58"/>
+      <c r="E11" s="47"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -2130,10 +2300,10 @@
       <c r="E16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="56" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="17" t="s">
@@ -2142,7 +2312,7 @@
       <c r="I16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="19" t="s">
         <v>34</v>
       </c>
       <c r="K16" t="s">
@@ -2150,27 +2320,27 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="8">
         <f>SUM(G16:G16)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="43">
+      <c r="H17" s="21">
         <f>SUM(H16:H16)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="43">
+      <c r="I17" s="21">
         <f>SUM(I16:I16)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="44">
+      <c r="J17" s="22">
         <f>SUM(J16:J16)</f>
         <v>0</v>
       </c>
@@ -2201,7 +2371,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="16"/>
       <c r="K19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2236,58 +2406,58 @@
         <v>5</v>
       </c>
       <c r="K20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36"/>
+      <c r="K21" t="s">
         <v>182</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="32"/>
-      <c r="K21" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="8">
         <f>SUM(G21:G21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="43">
+      <c r="H22" s="21">
         <f>SUM(H21:H21)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="43">
+      <c r="I22" s="21">
         <f>SUM(I21:I21)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="44">
+      <c r="J22" s="22">
         <f>SUM(J21:J21)</f>
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2360,10 +2530,10 @@
       <c r="E26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="56" t="s">
         <v>42</v>
       </c>
       <c r="H26" s="17" t="s">
@@ -2372,7 +2542,7 @@
       <c r="I26" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="J26" s="35" t="s">
+      <c r="J26" s="19" t="s">
         <v>45</v>
       </c>
       <c r="K26" t="s">
@@ -2380,27 +2550,27 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="8">
         <f>SUM(G26:G26)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="43">
+      <c r="H27" s="21">
         <f>SUM(H26:H26)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="43">
+      <c r="I27" s="21">
         <f>SUM(I26:I26)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="44">
+      <c r="J27" s="22">
         <f>SUM(J26:J26)</f>
         <v>0</v>
       </c>
@@ -2491,10 +2661,10 @@
       <c r="E31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="F31" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="56" t="s">
         <v>55</v>
       </c>
       <c r="H31" s="17" t="s">
@@ -2503,7 +2673,7 @@
       <c r="I31" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J31" s="35" t="s">
+      <c r="J31" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K31" t="s">
@@ -2511,27 +2681,27 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="8">
         <f>SUM(G31:G31)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="43">
+      <c r="H32" s="21">
         <f>SUM(H31:H31)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="43">
+      <c r="I32" s="21">
         <f>SUM(I31:I31)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="44">
+      <c r="J32" s="22">
         <f>SUM(J31:J31)</f>
         <v>0</v>
       </c>
@@ -2622,10 +2792,10 @@
       <c r="E36" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="56" t="s">
         <v>67</v>
       </c>
       <c r="H36" s="17" t="s">
@@ -2634,7 +2804,7 @@
       <c r="I36" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="J36" s="35" t="s">
+      <c r="J36" s="19" t="s">
         <v>70</v>
       </c>
       <c r="K36" t="s">
@@ -2642,27 +2812,27 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
       <c r="G37" s="8">
         <f>SUM(G36:G36)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="43">
+      <c r="H37" s="21">
         <f>SUM(H36:H36)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="43">
+      <c r="I37" s="21">
         <f>SUM(I36:I36)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="44">
+      <c r="J37" s="22">
         <f>SUM(J36:J36)</f>
         <v>0</v>
       </c>
@@ -2753,10 +2923,10 @@
       <c r="E41" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="F41" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="56" t="s">
         <v>80</v>
       </c>
       <c r="H41" s="17" t="s">
@@ -2765,7 +2935,7 @@
       <c r="I41" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="J41" s="35" t="s">
+      <c r="J41" s="19" t="s">
         <v>83</v>
       </c>
       <c r="K41" t="s">
@@ -2773,27 +2943,27 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
       <c r="G42" s="8">
         <f>SUM(G41:G41)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="45">
+      <c r="H42" s="24">
         <f>SUM(H41:H41)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="45">
+      <c r="I42" s="24">
         <f>SUM(I41:I41)</f>
         <v>0</v>
       </c>
-      <c r="J42" s="46">
+      <c r="J42" s="25">
         <f>SUM(J41:J41)</f>
         <v>0</v>
       </c>
@@ -2884,10 +3054,10 @@
       <c r="E46" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G46" s="56" t="s">
         <v>92</v>
       </c>
       <c r="H46" s="17" t="s">
@@ -2896,7 +3066,7 @@
       <c r="I46" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="J46" s="35" t="s">
+      <c r="J46" s="19" t="s">
         <v>95</v>
       </c>
       <c r="K46" t="s">
@@ -2904,27 +3074,27 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
       <c r="G47" s="8">
         <f>SUM(G46:G46)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="45">
+      <c r="H47" s="24">
         <f>SUM(H46:H46)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="45">
+      <c r="I47" s="24">
         <f>SUM(I46:I46)</f>
         <v>0</v>
       </c>
-      <c r="J47" s="46">
+      <c r="J47" s="25">
         <f>SUM(J46:J46)</f>
         <v>0</v>
       </c>
@@ -3015,10 +3185,10 @@
       <c r="E51" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="34" t="s">
+      <c r="F51" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="G51" s="18" t="s">
+      <c r="G51" s="56" t="s">
         <v>104</v>
       </c>
       <c r="H51" s="17" t="s">
@@ -3027,7 +3197,7 @@
       <c r="I51" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="J51" s="35" t="s">
+      <c r="J51" s="19" t="s">
         <v>107</v>
       </c>
       <c r="K51" t="s">
@@ -3035,27 +3205,27 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
       <c r="G52" s="8">
         <f>SUM(G51:G51)</f>
         <v>0</v>
       </c>
-      <c r="H52" s="45">
+      <c r="H52" s="24">
         <f>SUM(H51:H51)</f>
         <v>0</v>
       </c>
-      <c r="I52" s="45">
+      <c r="I52" s="24">
         <f>SUM(I51:I51)</f>
         <v>0</v>
       </c>
-      <c r="J52" s="46">
+      <c r="J52" s="25">
         <f>SUM(J51:J51)</f>
         <v>0</v>
       </c>
@@ -3146,10 +3316,10 @@
       <c r="E56" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F56" s="34" t="s">
+      <c r="F56" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="G56" s="18" t="s">
+      <c r="G56" s="56" t="s">
         <v>116</v>
       </c>
       <c r="H56" s="17" t="s">
@@ -3158,7 +3328,7 @@
       <c r="I56" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="J56" s="35" t="s">
+      <c r="J56" s="19" t="s">
         <v>119</v>
       </c>
       <c r="K56" t="s">
@@ -3166,27 +3336,27 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
       <c r="G57" s="8">
         <f>SUM(G56:G56)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="45">
+      <c r="H57" s="24">
         <f>SUM(H56:H56)</f>
         <v>0</v>
       </c>
-      <c r="I57" s="45">
+      <c r="I57" s="24">
         <f>SUM(I56:I56)</f>
         <v>0</v>
       </c>
-      <c r="J57" s="46">
+      <c r="J57" s="25">
         <f>SUM(J56:J56)</f>
         <v>0</v>
       </c>
@@ -3277,10 +3447,10 @@
       <c r="E61" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F61" s="34" t="s">
+      <c r="F61" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="G61" s="18" t="s">
+      <c r="G61" s="56" t="s">
         <v>128</v>
       </c>
       <c r="H61" s="17" t="s">
@@ -3289,7 +3459,7 @@
       <c r="I61" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="J61" s="35" t="s">
+      <c r="J61" s="19" t="s">
         <v>131</v>
       </c>
       <c r="K61" t="s">
@@ -3297,27 +3467,27 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
       <c r="G62" s="8">
         <f>SUM(G61:G61)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="45">
+      <c r="H62" s="24">
         <f>SUM(H61:H61)</f>
         <v>0</v>
       </c>
-      <c r="I62" s="45">
+      <c r="I62" s="24">
         <f>SUM(I61:I61)</f>
         <v>0</v>
       </c>
-      <c r="J62" s="46">
+      <c r="J62" s="25">
         <f>SUM(J61:J61)</f>
         <v>0</v>
       </c>
@@ -3408,10 +3578,10 @@
       <c r="E66" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F66" s="34" t="s">
+      <c r="F66" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="G66" s="18" t="s">
+      <c r="G66" s="56" t="s">
         <v>140</v>
       </c>
       <c r="H66" s="17" t="s">
@@ -3420,7 +3590,7 @@
       <c r="I66" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J66" s="35" t="s">
+      <c r="J66" s="19" t="s">
         <v>143</v>
       </c>
       <c r="K66" t="s">
@@ -3428,27 +3598,27 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
       <c r="G67" s="8">
         <f>SUM(G66:G66)</f>
         <v>0</v>
       </c>
-      <c r="H67" s="45">
+      <c r="H67" s="24">
         <f>SUM(H66:H66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="45">
+      <c r="I67" s="24">
         <f>SUM(I66:I66)</f>
         <v>0</v>
       </c>
-      <c r="J67" s="46">
+      <c r="J67" s="25">
         <f>SUM(J66:J66)</f>
         <v>0</v>
       </c>
@@ -3539,10 +3709,10 @@
       <c r="E71" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F71" s="34" t="s">
+      <c r="F71" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G71" s="18" t="s">
+      <c r="G71" s="56" t="s">
         <v>152</v>
       </c>
       <c r="H71" s="17" t="s">
@@ -3551,7 +3721,7 @@
       <c r="I71" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="J71" s="35" t="s">
+      <c r="J71" s="19" t="s">
         <v>155</v>
       </c>
       <c r="K71" t="s">
@@ -3559,27 +3729,27 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="20" t="s">
+      <c r="A72" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
       <c r="G72" s="8">
         <f>SUM(G71:G71)</f>
         <v>0</v>
       </c>
-      <c r="H72" s="45">
+      <c r="H72" s="24">
         <f>SUM(H71:H71)</f>
         <v>0</v>
       </c>
-      <c r="I72" s="45">
+      <c r="I72" s="24">
         <f>SUM(I71:I71)</f>
         <v>0</v>
       </c>
-      <c r="J72" s="46">
+      <c r="J72" s="25">
         <f>SUM(J71:J71)</f>
         <v>0</v>
       </c>
@@ -3602,12 +3772,12 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
       <c r="D74" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
@@ -3616,7 +3786,7 @@
       <c r="I74" s="14"/>
       <c r="J74" s="16"/>
       <c r="K74" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
@@ -3651,7 +3821,7 @@
         <v>5</v>
       </c>
       <c r="K75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
@@ -3659,63 +3829,63 @@
         <v>1</v>
       </c>
       <c r="B76" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="D76" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="E76" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="F76" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="F76" s="34" t="s">
+      <c r="G76" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="G76" s="18" t="s">
+      <c r="H76" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="H76" s="17" t="s">
+      <c r="I76" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="I76" s="17" t="s">
+      <c r="J76" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="J76" s="35" t="s">
-        <v>196</v>
-      </c>
       <c r="K76" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
       <c r="G77" s="8">
         <f>SUM(G76:G76)</f>
         <v>0</v>
       </c>
-      <c r="H77" s="43">
+      <c r="H77" s="21">
         <f>SUM(H76:H76)</f>
         <v>0</v>
       </c>
-      <c r="I77" s="43">
+      <c r="I77" s="21">
         <f>SUM(I76:I76)</f>
         <v>0</v>
       </c>
-      <c r="J77" s="44">
+      <c r="J77" s="22">
         <f>SUM(J76:J76)</f>
         <v>0</v>
       </c>
       <c r="K77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
@@ -3728,17 +3898,17 @@
       <c r="I78" s="11"/>
       <c r="J78" s="9"/>
       <c r="K78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E79" s="14"/>
       <c r="F79" s="14"/>
@@ -3747,7 +3917,7 @@
       <c r="I79" s="14"/>
       <c r="J79" s="16"/>
       <c r="K79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
@@ -3782,7 +3952,7 @@
         <v>5</v>
       </c>
       <c r="K80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
@@ -3790,63 +3960,63 @@
         <v>1</v>
       </c>
       <c r="B81" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="F81" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="F81" s="34" t="s">
+      <c r="G81" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="G81" s="18" t="s">
+      <c r="H81" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="H81" s="17" t="s">
+      <c r="I81" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="I81" s="17" t="s">
+      <c r="J81" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="J81" s="35" t="s">
-        <v>208</v>
-      </c>
       <c r="K81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
       <c r="G82" s="8">
         <f>SUM(G81:G81)</f>
         <v>0</v>
       </c>
-      <c r="H82" s="43">
+      <c r="H82" s="21">
         <f>SUM(H81:H81)</f>
         <v>0</v>
       </c>
-      <c r="I82" s="43">
+      <c r="I82" s="21">
         <f>SUM(I81:I81)</f>
         <v>0</v>
       </c>
-      <c r="J82" s="44">
+      <c r="J82" s="22">
         <f>SUM(J81:J81)</f>
         <v>0</v>
       </c>
       <c r="K82" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
@@ -3859,17 +4029,17 @@
       <c r="I83" s="11"/>
       <c r="J83" s="9"/>
       <c r="K83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
       <c r="D84" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E84" s="14"/>
       <c r="F84" s="14"/>
@@ -3878,7 +4048,7 @@
       <c r="I84" s="14"/>
       <c r="J84" s="16"/>
       <c r="K84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
@@ -3913,7 +4083,7 @@
         <v>5</v>
       </c>
       <c r="K85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
@@ -3921,63 +4091,63 @@
         <v>1</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="D86" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="E86" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="F86" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="F86" s="34" t="s">
+      <c r="G86" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="G86" s="18" t="s">
+      <c r="H86" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="H86" s="17" t="s">
+      <c r="I86" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="I86" s="17" t="s">
+      <c r="J86" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="J86" s="35" t="s">
-        <v>220</v>
-      </c>
       <c r="K86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A87" s="20" t="s">
+      <c r="A87" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
       <c r="G87" s="8">
         <f>SUM(G86:G86)</f>
         <v>0</v>
       </c>
-      <c r="H87" s="43">
+      <c r="H87" s="21">
         <f>SUM(H86:H86)</f>
         <v>0</v>
       </c>
-      <c r="I87" s="43">
+      <c r="I87" s="21">
         <f>SUM(I86:I86)</f>
         <v>0</v>
       </c>
-      <c r="J87" s="44">
+      <c r="J87" s="22">
         <f>SUM(J86:J86)</f>
         <v>0</v>
       </c>
       <c r="K87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
@@ -3990,17 +4160,17 @@
       <c r="I88" s="11"/>
       <c r="J88" s="9"/>
       <c r="K88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
       <c r="D89" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="14"/>
@@ -4009,7 +4179,7 @@
       <c r="I89" s="14"/>
       <c r="J89" s="16"/>
       <c r="K89" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
@@ -4044,7 +4214,7 @@
         <v>5</v>
       </c>
       <c r="K90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
@@ -4052,63 +4222,63 @@
         <v>1</v>
       </c>
       <c r="B91" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="D91" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="E91" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="F91" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="F91" s="34" t="s">
+      <c r="G91" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="G91" s="18" t="s">
+      <c r="H91" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="H91" s="17" t="s">
+      <c r="I91" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="I91" s="17" t="s">
+      <c r="J91" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="J91" s="35" t="s">
-        <v>232</v>
-      </c>
       <c r="K91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="20" t="s">
+      <c r="A92" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
       <c r="G92" s="8">
         <f>SUM(G91:G91)</f>
         <v>0</v>
       </c>
-      <c r="H92" s="45">
+      <c r="H92" s="24">
         <f>SUM(H91:H91)</f>
         <v>0</v>
       </c>
-      <c r="I92" s="45">
+      <c r="I92" s="24">
         <f>SUM(I91:I91)</f>
         <v>0</v>
       </c>
-      <c r="J92" s="46">
+      <c r="J92" s="25">
         <f>SUM(J91:J91)</f>
         <v>0</v>
       </c>
       <c r="K92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
@@ -4121,17 +4291,17 @@
       <c r="I93" s="11"/>
       <c r="J93" s="9"/>
       <c r="K93" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
       <c r="D94" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E94" s="14"/>
       <c r="F94" s="14"/>
@@ -4140,7 +4310,7 @@
       <c r="I94" s="14"/>
       <c r="J94" s="16"/>
       <c r="K94" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
@@ -4175,7 +4345,7 @@
         <v>5</v>
       </c>
       <c r="K95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
@@ -4183,63 +4353,63 @@
         <v>1</v>
       </c>
       <c r="B96" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="D96" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="E96" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E96" s="6" t="s">
+      <c r="F96" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="F96" s="34" t="s">
+      <c r="G96" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="G96" s="18" t="s">
+      <c r="H96" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="H96" s="17" t="s">
+      <c r="I96" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="I96" s="17" t="s">
+      <c r="J96" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="J96" s="35" t="s">
-        <v>244</v>
-      </c>
       <c r="K96" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="20" t="s">
+      <c r="A97" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="21"/>
-      <c r="C97" s="21"/>
-      <c r="D97" s="21"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="37"/>
       <c r="G97" s="8">
         <f>SUM(G96:G96)</f>
         <v>0</v>
       </c>
-      <c r="H97" s="45">
+      <c r="H97" s="24">
         <f>SUM(H96:H96)</f>
         <v>0</v>
       </c>
-      <c r="I97" s="45">
+      <c r="I97" s="24">
         <f>SUM(I96:I96)</f>
         <v>0</v>
       </c>
-      <c r="J97" s="46">
+      <c r="J97" s="25">
         <f>SUM(J96:J96)</f>
         <v>0</v>
       </c>
       <c r="K97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
@@ -4252,17 +4422,17 @@
       <c r="I98" s="11"/>
       <c r="J98" s="9"/>
       <c r="K98" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
       <c r="D99" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E99" s="14"/>
       <c r="F99" s="14"/>
@@ -4271,7 +4441,7 @@
       <c r="I99" s="14"/>
       <c r="J99" s="16"/>
       <c r="K99" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
@@ -4306,7 +4476,7 @@
         <v>5</v>
       </c>
       <c r="K100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
@@ -4314,63 +4484,63 @@
         <v>1</v>
       </c>
       <c r="B101" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="D101" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="E101" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="F101" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="F101" s="34" t="s">
+      <c r="G101" s="56" t="s">
         <v>252</v>
       </c>
-      <c r="G101" s="18" t="s">
+      <c r="H101" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="H101" s="17" t="s">
+      <c r="I101" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="I101" s="17" t="s">
+      <c r="J101" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="J101" s="35" t="s">
-        <v>256</v>
-      </c>
       <c r="K101" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A102" s="20" t="s">
+      <c r="A102" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="21"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
-      <c r="E102" s="21"/>
-      <c r="F102" s="21"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
       <c r="G102" s="8">
         <f>SUM(G101:G101)</f>
         <v>0</v>
       </c>
-      <c r="H102" s="45">
+      <c r="H102" s="24">
         <f>SUM(H101:H101)</f>
         <v>0</v>
       </c>
-      <c r="I102" s="45">
+      <c r="I102" s="24">
         <f>SUM(I101:I101)</f>
         <v>0</v>
       </c>
-      <c r="J102" s="46">
+      <c r="J102" s="25">
         <f>SUM(J101:J101)</f>
         <v>0</v>
       </c>
       <c r="K102" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
@@ -4383,17 +4553,17 @@
       <c r="I103" s="11"/>
       <c r="J103" s="9"/>
       <c r="K103" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B104" s="14"/>
       <c r="C104" s="14"/>
       <c r="D104" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E104" s="14"/>
       <c r="F104" s="14"/>
@@ -4402,7 +4572,7 @@
       <c r="I104" s="14"/>
       <c r="J104" s="16"/>
       <c r="K104" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
@@ -4437,7 +4607,7 @@
         <v>5</v>
       </c>
       <c r="K105" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
@@ -4445,63 +4615,63 @@
         <v>1</v>
       </c>
       <c r="B106" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C106" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="D106" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="D106" s="6" t="s">
+      <c r="E106" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="E106" s="6" t="s">
+      <c r="F106" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="F106" s="34" t="s">
+      <c r="G106" s="56" t="s">
         <v>264</v>
       </c>
-      <c r="G106" s="18" t="s">
+      <c r="H106" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="H106" s="17" t="s">
+      <c r="I106" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="I106" s="17" t="s">
+      <c r="J106" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="J106" s="35" t="s">
-        <v>268</v>
-      </c>
       <c r="K106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A107" s="20" t="s">
+      <c r="A107" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B107" s="21"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
+      <c r="B107" s="37"/>
+      <c r="C107" s="37"/>
+      <c r="D107" s="37"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
       <c r="G107" s="8">
         <f>SUM(G106:G106)</f>
         <v>0</v>
       </c>
-      <c r="H107" s="45">
+      <c r="H107" s="24">
         <f>SUM(H106:H106)</f>
         <v>0</v>
       </c>
-      <c r="I107" s="45">
+      <c r="I107" s="24">
         <f>SUM(I106:I106)</f>
         <v>0</v>
       </c>
-      <c r="J107" s="46">
+      <c r="J107" s="25">
         <f>SUM(J106:J106)</f>
         <v>0</v>
       </c>
       <c r="K107" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
@@ -4514,17 +4684,17 @@
       <c r="I108" s="11"/>
       <c r="J108" s="9"/>
       <c r="K108" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B109" s="14"/>
       <c r="C109" s="14"/>
       <c r="D109" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E109" s="14"/>
       <c r="F109" s="14"/>
@@ -4533,7 +4703,7 @@
       <c r="I109" s="14"/>
       <c r="J109" s="16"/>
       <c r="K109" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
@@ -4568,7 +4738,7 @@
         <v>5</v>
       </c>
       <c r="K110" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
@@ -4576,63 +4746,63 @@
         <v>1</v>
       </c>
       <c r="B111" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C111" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="D111" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="E111" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="E111" s="6" t="s">
+      <c r="F111" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="F111" s="34" t="s">
+      <c r="G111" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="G111" s="18" t="s">
+      <c r="H111" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="H111" s="17" t="s">
+      <c r="I111" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="I111" s="17" t="s">
+      <c r="J111" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="J111" s="35" t="s">
-        <v>280</v>
-      </c>
       <c r="K111" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A112" s="20" t="s">
+      <c r="A112" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B112" s="21"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="21"/>
-      <c r="E112" s="21"/>
-      <c r="F112" s="21"/>
+      <c r="B112" s="37"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="37"/>
       <c r="G112" s="8">
         <f>SUM(G111:G111)</f>
         <v>0</v>
       </c>
-      <c r="H112" s="45">
+      <c r="H112" s="24">
         <f>SUM(H111:H111)</f>
         <v>0</v>
       </c>
-      <c r="I112" s="45">
+      <c r="I112" s="24">
         <f>SUM(I111:I111)</f>
         <v>0</v>
       </c>
-      <c r="J112" s="46">
+      <c r="J112" s="25">
         <f>SUM(J111:J111)</f>
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
@@ -4645,17 +4815,17 @@
       <c r="I113" s="11"/>
       <c r="J113" s="9"/>
       <c r="K113" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B114" s="14"/>
       <c r="C114" s="14"/>
       <c r="D114" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E114" s="14"/>
       <c r="F114" s="14"/>
@@ -4664,7 +4834,7 @@
       <c r="I114" s="14"/>
       <c r="J114" s="16"/>
       <c r="K114" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.3">
@@ -4699,7 +4869,7 @@
         <v>5</v>
       </c>
       <c r="K115" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
@@ -4707,63 +4877,63 @@
         <v>1</v>
       </c>
       <c r="B116" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C116" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C116" s="6" t="s">
+      <c r="D116" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="D116" s="6" t="s">
+      <c r="E116" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="E116" s="6" t="s">
+      <c r="F116" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="F116" s="34" t="s">
+      <c r="G116" s="56" t="s">
         <v>288</v>
       </c>
-      <c r="G116" s="18" t="s">
+      <c r="H116" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="H116" s="17" t="s">
+      <c r="I116" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="I116" s="17" t="s">
+      <c r="J116" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="J116" s="35" t="s">
-        <v>292</v>
-      </c>
       <c r="K116" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A117" s="20" t="s">
+      <c r="A117" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B117" s="21"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="21"/>
-      <c r="E117" s="21"/>
-      <c r="F117" s="21"/>
+      <c r="B117" s="37"/>
+      <c r="C117" s="37"/>
+      <c r="D117" s="37"/>
+      <c r="E117" s="37"/>
+      <c r="F117" s="37"/>
       <c r="G117" s="8">
         <f>SUM(G116:G116)</f>
         <v>0</v>
       </c>
-      <c r="H117" s="45">
+      <c r="H117" s="24">
         <f>SUM(H116:H116)</f>
         <v>0</v>
       </c>
-      <c r="I117" s="45">
+      <c r="I117" s="24">
         <f>SUM(I116:I116)</f>
         <v>0</v>
       </c>
-      <c r="J117" s="46">
+      <c r="J117" s="25">
         <f>SUM(J116:J116)</f>
         <v>0</v>
       </c>
       <c r="K117" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.3">
@@ -4776,17 +4946,17 @@
       <c r="I118" s="11"/>
       <c r="J118" s="9"/>
       <c r="K118" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="14"/>
       <c r="D119" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E119" s="14"/>
       <c r="F119" s="14"/>
@@ -4795,7 +4965,7 @@
       <c r="I119" s="14"/>
       <c r="J119" s="16"/>
       <c r="K119" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
@@ -4830,7 +5000,7 @@
         <v>5</v>
       </c>
       <c r="K120" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.3">
@@ -4838,63 +5008,63 @@
         <v>1</v>
       </c>
       <c r="B121" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C121" s="6" t="s">
+      <c r="D121" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="D121" s="6" t="s">
+      <c r="E121" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="E121" s="6" t="s">
+      <c r="F121" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="F121" s="34" t="s">
+      <c r="G121" s="56" t="s">
         <v>300</v>
       </c>
-      <c r="G121" s="18" t="s">
+      <c r="H121" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="H121" s="17" t="s">
+      <c r="I121" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="I121" s="17" t="s">
+      <c r="J121" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="J121" s="35" t="s">
-        <v>304</v>
-      </c>
       <c r="K121" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122" s="20" t="s">
+      <c r="A122" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B122" s="21"/>
-      <c r="C122" s="21"/>
-      <c r="D122" s="21"/>
-      <c r="E122" s="21"/>
-      <c r="F122" s="21"/>
+      <c r="B122" s="37"/>
+      <c r="C122" s="37"/>
+      <c r="D122" s="37"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="37"/>
       <c r="G122" s="8">
         <f>SUM(G121:G121)</f>
         <v>0</v>
       </c>
-      <c r="H122" s="45">
+      <c r="H122" s="24">
         <f>SUM(H121:H121)</f>
         <v>0</v>
       </c>
-      <c r="I122" s="45">
+      <c r="I122" s="24">
         <f>SUM(I121:I121)</f>
         <v>0</v>
       </c>
-      <c r="J122" s="46">
+      <c r="J122" s="25">
         <f>SUM(J121:J121)</f>
         <v>0</v>
       </c>
       <c r="K122" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.3">
@@ -4907,17 +5077,17 @@
       <c r="I123" s="11"/>
       <c r="J123" s="9"/>
       <c r="K123" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B124" s="14"/>
       <c r="C124" s="14"/>
       <c r="D124" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E124" s="14"/>
       <c r="F124" s="14"/>
@@ -4926,7 +5096,7 @@
       <c r="I124" s="14"/>
       <c r="J124" s="16"/>
       <c r="K124" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
@@ -4961,7 +5131,7 @@
         <v>5</v>
       </c>
       <c r="K125" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
@@ -4969,63 +5139,63 @@
         <v>1</v>
       </c>
       <c r="B126" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C126" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="D126" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="D126" s="6" t="s">
+      <c r="E126" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="E126" s="6" t="s">
+      <c r="F126" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="F126" s="34" t="s">
+      <c r="G126" s="56" t="s">
         <v>312</v>
       </c>
-      <c r="G126" s="18" t="s">
+      <c r="H126" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="H126" s="17" t="s">
+      <c r="I126" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="I126" s="17" t="s">
+      <c r="J126" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="J126" s="35" t="s">
-        <v>316</v>
-      </c>
       <c r="K126" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A127" s="20" t="s">
+      <c r="A127" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B127" s="21"/>
-      <c r="C127" s="21"/>
-      <c r="D127" s="21"/>
-      <c r="E127" s="21"/>
-      <c r="F127" s="21"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="37"/>
+      <c r="D127" s="37"/>
+      <c r="E127" s="37"/>
+      <c r="F127" s="37"/>
       <c r="G127" s="8">
         <f>SUM(G126:G126)</f>
         <v>0</v>
       </c>
-      <c r="H127" s="43">
+      <c r="H127" s="21">
         <f>SUM(H126:H126)</f>
         <v>0</v>
       </c>
-      <c r="I127" s="43">
+      <c r="I127" s="21">
         <f>SUM(I126:I126)</f>
         <v>0</v>
       </c>
-      <c r="J127" s="44">
+      <c r="J127" s="22">
         <f>SUM(J126:J126)</f>
         <v>0</v>
       </c>
       <c r="K127" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.3">
@@ -5038,17 +5208,17 @@
       <c r="I128" s="11"/>
       <c r="J128" s="9"/>
       <c r="K128" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B129" s="14"/>
       <c r="C129" s="14"/>
       <c r="D129" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E129" s="14"/>
       <c r="F129" s="14"/>
@@ -5057,7 +5227,7 @@
       <c r="I129" s="14"/>
       <c r="J129" s="16"/>
       <c r="K129" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.3">
@@ -5092,7 +5262,7 @@
         <v>5</v>
       </c>
       <c r="K130" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.3">
@@ -5100,63 +5270,63 @@
         <v>1</v>
       </c>
       <c r="B131" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C131" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="C131" s="6" t="s">
+      <c r="D131" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="D131" s="6" t="s">
+      <c r="E131" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="E131" s="6" t="s">
+      <c r="F131" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="F131" s="34" t="s">
+      <c r="G131" s="56" t="s">
         <v>324</v>
       </c>
-      <c r="G131" s="18" t="s">
+      <c r="H131" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="H131" s="17" t="s">
+      <c r="I131" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="I131" s="17" t="s">
+      <c r="J131" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="J131" s="35" t="s">
-        <v>328</v>
-      </c>
       <c r="K131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A132" s="20" t="s">
+      <c r="A132" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B132" s="21"/>
-      <c r="C132" s="21"/>
-      <c r="D132" s="21"/>
-      <c r="E132" s="21"/>
-      <c r="F132" s="21"/>
+      <c r="B132" s="37"/>
+      <c r="C132" s="37"/>
+      <c r="D132" s="37"/>
+      <c r="E132" s="37"/>
+      <c r="F132" s="37"/>
       <c r="G132" s="8">
         <f>SUM(G131:G131)</f>
         <v>0</v>
       </c>
-      <c r="H132" s="43">
+      <c r="H132" s="21">
         <f>SUM(H131:H131)</f>
         <v>0</v>
       </c>
-      <c r="I132" s="43">
+      <c r="I132" s="21">
         <f>SUM(I131:I131)</f>
         <v>0</v>
       </c>
-      <c r="J132" s="44">
+      <c r="J132" s="22">
         <f>SUM(J131:J131)</f>
         <v>0</v>
       </c>
       <c r="K132" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
@@ -5169,17 +5339,17 @@
       <c r="I133" s="11"/>
       <c r="J133" s="9"/>
       <c r="K133" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B134" s="14"/>
       <c r="C134" s="14"/>
       <c r="D134" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E134" s="14"/>
       <c r="F134" s="14"/>
@@ -5188,7 +5358,7 @@
       <c r="I134" s="14"/>
       <c r="J134" s="16"/>
       <c r="K134" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.3">
@@ -5223,7 +5393,7 @@
         <v>5</v>
       </c>
       <c r="K135" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.3">
@@ -5231,63 +5401,63 @@
         <v>1</v>
       </c>
       <c r="B136" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C136" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="D136" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="D136" s="6" t="s">
+      <c r="E136" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="E136" s="6" t="s">
+      <c r="F136" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="F136" s="34" t="s">
+      <c r="G136" s="56" t="s">
         <v>336</v>
       </c>
-      <c r="G136" s="18" t="s">
+      <c r="H136" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="H136" s="17" t="s">
+      <c r="I136" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="I136" s="17" t="s">
+      <c r="J136" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="J136" s="35" t="s">
-        <v>340</v>
-      </c>
       <c r="K136" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A137" s="20" t="s">
+      <c r="A137" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B137" s="21"/>
-      <c r="C137" s="21"/>
-      <c r="D137" s="21"/>
-      <c r="E137" s="21"/>
-      <c r="F137" s="21"/>
+      <c r="B137" s="37"/>
+      <c r="C137" s="37"/>
+      <c r="D137" s="37"/>
+      <c r="E137" s="37"/>
+      <c r="F137" s="37"/>
       <c r="G137" s="8">
         <f>SUM(G136:G136)</f>
         <v>0</v>
       </c>
-      <c r="H137" s="43">
+      <c r="H137" s="21">
         <f>SUM(H136:H136)</f>
         <v>0</v>
       </c>
-      <c r="I137" s="43">
+      <c r="I137" s="21">
         <f>SUM(I136:I136)</f>
         <v>0</v>
       </c>
-      <c r="J137" s="44">
+      <c r="J137" s="22">
         <f>SUM(J136:J136)</f>
         <v>0</v>
       </c>
       <c r="K137" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.3">
@@ -5300,17 +5470,17 @@
       <c r="I138" s="11"/>
       <c r="J138" s="9"/>
       <c r="K138" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="14"/>
       <c r="D139" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E139" s="14"/>
       <c r="F139" s="14"/>
@@ -5319,7 +5489,7 @@
       <c r="I139" s="14"/>
       <c r="J139" s="16"/>
       <c r="K139" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.3">
@@ -5354,7 +5524,7 @@
         <v>5</v>
       </c>
       <c r="K140" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.3">
@@ -5362,63 +5532,63 @@
         <v>1</v>
       </c>
       <c r="B141" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C141" s="6" t="s">
+      <c r="D141" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="D141" s="6" t="s">
+      <c r="E141" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="E141" s="6" t="s">
+      <c r="F141" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="F141" s="34" t="s">
+      <c r="G141" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="G141" s="18" t="s">
+      <c r="H141" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="H141" s="17" t="s">
+      <c r="I141" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I141" s="17" t="s">
+      <c r="J141" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="J141" s="35" t="s">
-        <v>352</v>
-      </c>
       <c r="K141" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A142" s="20" t="s">
+      <c r="A142" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B142" s="21"/>
-      <c r="C142" s="21"/>
-      <c r="D142" s="21"/>
-      <c r="E142" s="21"/>
-      <c r="F142" s="21"/>
+      <c r="B142" s="37"/>
+      <c r="C142" s="37"/>
+      <c r="D142" s="37"/>
+      <c r="E142" s="37"/>
+      <c r="F142" s="37"/>
       <c r="G142" s="8">
         <f>SUM(G141:G141)</f>
         <v>0</v>
       </c>
-      <c r="H142" s="45">
+      <c r="H142" s="24">
         <f>SUM(H141:H141)</f>
         <v>0</v>
       </c>
-      <c r="I142" s="45">
+      <c r="I142" s="24">
         <f>SUM(I141:I141)</f>
         <v>0</v>
       </c>
-      <c r="J142" s="46">
+      <c r="J142" s="25">
         <f>SUM(J141:J141)</f>
         <v>0</v>
       </c>
       <c r="K142" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.3">
@@ -5431,7 +5601,7 @@
       <c r="I143" s="11"/>
       <c r="J143" s="9"/>
       <c r="K143" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.3">
@@ -5456,10 +5626,10 @@
       <c r="A145" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B145" s="26" t="s">
+      <c r="B145" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C145" s="26"/>
+      <c r="C145" s="30"/>
       <c r="D145" s="3" t="s">
         <v>11</v>
       </c>
@@ -5477,20 +5647,20 @@
       <c r="J145" s="9"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A146" s="49">
+      <c r="A146" s="27">
         <v>1</v>
       </c>
-      <c r="B146" s="50" t="s">
+      <c r="B146" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="C146" s="50"/>
-      <c r="D146" s="51" t="s">
+      <c r="C146" s="31"/>
+      <c r="D146" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="E146" s="51" t="s">
+      <c r="E146" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="F146" s="52" t="s">
+      <c r="F146" s="29" t="s">
         <v>177</v>
       </c>
       <c r="G146" t="s">
@@ -5514,17 +5684,17 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B148" s="14"/>
       <c r="C148" s="14"/>
       <c r="D148" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E148" s="14"/>
       <c r="F148" s="16"/>
       <c r="G148" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H148" s="11"/>
       <c r="I148" s="11"/>
@@ -5534,10 +5704,10 @@
       <c r="A149" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B149" s="26" t="s">
+      <c r="B149" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C149" s="26"/>
+      <c r="C149" s="30"/>
       <c r="D149" s="3" t="s">
         <v>11</v>
       </c>
@@ -5548,31 +5718,31 @@
         <v>164</v>
       </c>
       <c r="G149" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H149" s="11"/>
       <c r="I149" s="11"/>
       <c r="J149" s="9"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A150" s="49">
+      <c r="A150" s="27">
         <v>1</v>
       </c>
-      <c r="B150" s="50" t="s">
+      <c r="B150" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="C150" s="31"/>
+      <c r="D150" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="C150" s="50"/>
-      <c r="D150" s="51" t="s">
+      <c r="E150" s="28" t="s">
         <v>357</v>
       </c>
-      <c r="E150" s="51" t="s">
+      <c r="F150" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="F150" s="52" t="s">
-        <v>359</v>
-      </c>
       <c r="G150" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H150" s="11"/>
       <c r="I150" s="11"/>
@@ -5584,7 +5754,7 @@
       <c r="E151" s="9"/>
       <c r="F151" s="11"/>
       <c r="G151" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H151" s="11"/>
       <c r="I151" s="11"/>
@@ -5592,17 +5762,17 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="14"/>
       <c r="D152" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E152" s="14"/>
       <c r="F152" s="16"/>
       <c r="G152" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
@@ -5612,10 +5782,10 @@
       <c r="A153" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B153" s="26" t="s">
+      <c r="B153" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C153" s="26"/>
+      <c r="C153" s="30"/>
       <c r="D153" s="3" t="s">
         <v>11</v>
       </c>
@@ -5626,31 +5796,31 @@
         <v>164</v>
       </c>
       <c r="G153" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H153" s="11"/>
       <c r="I153" s="11"/>
       <c r="J153" s="9"/>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A154" s="49">
+      <c r="A154" s="27">
         <v>1</v>
       </c>
-      <c r="B154" s="50" t="s">
+      <c r="B154" s="31" t="s">
+        <v>362</v>
+      </c>
+      <c r="C154" s="31"/>
+      <c r="D154" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="C154" s="50"/>
-      <c r="D154" s="51" t="s">
+      <c r="E154" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="E154" s="51" t="s">
+      <c r="F154" s="29" t="s">
         <v>365</v>
       </c>
-      <c r="F154" s="52" t="s">
-        <v>366</v>
-      </c>
       <c r="G154" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H154" s="11"/>
       <c r="I154" s="11"/>
@@ -5662,7 +5832,7 @@
       <c r="E155" s="9"/>
       <c r="F155" s="11"/>
       <c r="G155" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H155" s="11"/>
       <c r="I155" s="11"/>
@@ -5670,17 +5840,17 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B156" s="14"/>
       <c r="C156" s="14"/>
       <c r="D156" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E156" s="14"/>
       <c r="F156" s="16"/>
       <c r="G156" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H156" s="11"/>
       <c r="I156" s="11"/>
@@ -5690,10 +5860,10 @@
       <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B157" s="26" t="s">
+      <c r="B157" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C157" s="26"/>
+      <c r="C157" s="30"/>
       <c r="D157" s="3" t="s">
         <v>11</v>
       </c>
@@ -5704,31 +5874,31 @@
         <v>164</v>
       </c>
       <c r="G157" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H157" s="11"/>
       <c r="I157" s="11"/>
       <c r="J157" s="9"/>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A158" s="49">
+      <c r="A158" s="27">
         <v>1</v>
       </c>
-      <c r="B158" s="50" t="s">
+      <c r="B158" s="31" t="s">
+        <v>369</v>
+      </c>
+      <c r="C158" s="31"/>
+      <c r="D158" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="C158" s="50"/>
-      <c r="D158" s="51" t="s">
+      <c r="E158" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="E158" s="51" t="s">
+      <c r="F158" s="29" t="s">
         <v>372</v>
       </c>
-      <c r="F158" s="52" t="s">
-        <v>373</v>
-      </c>
       <c r="G158" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H158" s="11"/>
       <c r="I158" s="11"/>
@@ -5740,7 +5910,7 @@
       <c r="E159" s="9"/>
       <c r="F159" s="11"/>
       <c r="G159" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H159" s="11"/>
       <c r="I159" s="11"/>
@@ -5748,17 +5918,17 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B160" s="14"/>
       <c r="C160" s="14"/>
       <c r="D160" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E160" s="14"/>
       <c r="F160" s="16"/>
       <c r="G160" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H160" s="11"/>
       <c r="I160" s="11"/>
@@ -5768,10 +5938,10 @@
       <c r="A161" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B161" s="26" t="s">
+      <c r="B161" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C161" s="26"/>
+      <c r="C161" s="30"/>
       <c r="D161" s="3" t="s">
         <v>11</v>
       </c>
@@ -5782,31 +5952,31 @@
         <v>164</v>
       </c>
       <c r="G161" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H161" s="11"/>
       <c r="I161" s="11"/>
       <c r="J161" s="9"/>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A162" s="49">
+      <c r="A162" s="27">
         <v>1</v>
       </c>
-      <c r="B162" s="50" t="s">
+      <c r="B162" s="31" t="s">
+        <v>376</v>
+      </c>
+      <c r="C162" s="31"/>
+      <c r="D162" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="C162" s="50"/>
-      <c r="D162" s="51" t="s">
+      <c r="E162" s="28" t="s">
         <v>378</v>
       </c>
-      <c r="E162" s="51" t="s">
+      <c r="F162" s="29" t="s">
         <v>379</v>
       </c>
-      <c r="F162" s="52" t="s">
-        <v>380</v>
-      </c>
       <c r="G162" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I162" s="11"/>
       <c r="J162" s="9"/>
@@ -5817,125 +5987,832 @@
       <c r="E163" s="9"/>
       <c r="F163" s="11"/>
       <c r="G163" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I163" s="11"/>
       <c r="J163" s="9"/>
     </row>
     <row r="164" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
+      <c r="A164" s="53" t="s">
+        <v>381</v>
+      </c>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="11"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="9"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A165" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="B165" s="14"/>
+      <c r="C165" s="14"/>
+      <c r="D165" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="E165" s="14"/>
+      <c r="F165" s="14"/>
+      <c r="G165" s="14"/>
+      <c r="H165" s="14"/>
+      <c r="I165" s="16"/>
+      <c r="J165" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I166" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J166" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A167" s="5">
+        <v>1</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="F167" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="G167" s="56" t="s">
+        <v>390</v>
+      </c>
+      <c r="H167" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="I167" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="J167" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A168" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B168" s="37"/>
+      <c r="C168" s="37"/>
+      <c r="D168" s="37"/>
+      <c r="E168" s="37"/>
+      <c r="F168" s="37"/>
+      <c r="G168" s="8">
+        <f>SUM(G167:G167)</f>
+        <v>0</v>
+      </c>
+      <c r="H168" s="21">
+        <f>SUM(H167:H167)</f>
+        <v>0</v>
+      </c>
+      <c r="I168" s="22">
+        <f>SUM(I167:I167)</f>
+        <v>0</v>
+      </c>
+      <c r="J168" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J169" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A170" s="13" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="B170" s="14"/>
+      <c r="C170" s="14"/>
+      <c r="D170" s="13" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="E170" s="14"/>
+      <c r="F170" s="14"/>
+      <c r="G170" s="14"/>
+      <c r="H170" s="14"/>
+      <c r="I170" s="16"/>
+      <c r="J170" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A171" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H171" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I171" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J171" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A172" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="B172" s="54"/>
+      <c r="C172" s="54"/>
+      <c r="D172" s="54"/>
+      <c r="E172" s="54"/>
+      <c r="F172" s="54"/>
+      <c r="G172" s="54"/>
+      <c r="H172" s="54"/>
+      <c r="I172" s="55"/>
+      <c r="J172" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A173" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173" s="37"/>
+      <c r="C173" s="37"/>
+      <c r="D173" s="37"/>
+      <c r="E173" s="37"/>
+      <c r="F173" s="37"/>
+      <c r="G173" s="8">
+        <f>SUM(G172:G172)</f>
+        <v>0</v>
+      </c>
+      <c r="H173" s="21">
+        <f>SUM(H172:H172)</f>
+        <v>0</v>
+      </c>
+      <c r="I173" s="22">
+        <f>SUM(I172:I172)</f>
+        <v>0</v>
+      </c>
+      <c r="J173" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J174" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A175" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="B175" s="14"/>
+      <c r="C175" s="14"/>
+      <c r="D175" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="E175" s="14"/>
+      <c r="F175" s="14"/>
+      <c r="G175" s="14"/>
+      <c r="H175" s="14"/>
+      <c r="I175" s="16"/>
+      <c r="J175" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I176" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J176" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A177" s="5">
+        <v>1</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="D177" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="E177" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="F177" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="G177" s="56" t="s">
+        <v>402</v>
+      </c>
+      <c r="H177" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="I177" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="J177" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A178" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B178" s="37"/>
+      <c r="C178" s="37"/>
+      <c r="D178" s="37"/>
+      <c r="E178" s="37"/>
+      <c r="F178" s="37"/>
+      <c r="G178" s="8">
+        <f>SUM(G177:G177)</f>
+        <v>0</v>
+      </c>
+      <c r="H178" s="21">
+        <f>SUM(H177:H177)</f>
+        <v>0</v>
+      </c>
+      <c r="I178" s="22">
+        <f>SUM(I177:I177)</f>
+        <v>0</v>
+      </c>
+      <c r="J178" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A179" s="10"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="11"/>
+      <c r="G179" s="12"/>
+      <c r="H179" s="11"/>
+      <c r="I179" s="9"/>
+      <c r="J179" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A180" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="B180" s="14"/>
+      <c r="C180" s="14"/>
+      <c r="D180" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E180" s="14"/>
+      <c r="F180" s="14"/>
+      <c r="G180" s="14"/>
+      <c r="H180" s="14"/>
+      <c r="I180" s="16"/>
+      <c r="J180" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H181" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I181" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J181" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A182" s="5">
+        <v>1</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D182" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E182" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="F182" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="G182" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="H182" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="I182" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="J182" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A183" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B183" s="37"/>
+      <c r="C183" s="37"/>
+      <c r="D183" s="37"/>
+      <c r="E183" s="37"/>
+      <c r="F183" s="37"/>
+      <c r="G183" s="8">
+        <f>SUM(G182:G182)</f>
+        <v>0</v>
+      </c>
+      <c r="H183" s="21">
+        <f>SUM(H182:H182)</f>
+        <v>0</v>
+      </c>
+      <c r="I183" s="22">
+        <f>SUM(I182:I182)</f>
+        <v>0</v>
+      </c>
+      <c r="J183" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A184" s="10"/>
+      <c r="D184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="11"/>
+      <c r="G184" s="12"/>
+      <c r="H184" s="11"/>
+      <c r="I184" s="9"/>
+      <c r="J184" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A185" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="B185" s="14"/>
+      <c r="C185" s="14"/>
+      <c r="D185" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="E185" s="14"/>
+      <c r="F185" s="14"/>
+      <c r="G185" s="14"/>
+      <c r="H185" s="14"/>
+      <c r="I185" s="16"/>
+      <c r="J185" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I186" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J186" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A187" s="5">
+        <v>1</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="D187" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="F187" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G187" s="56" t="s">
+        <v>424</v>
+      </c>
+      <c r="H187" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="I187" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="J187" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A188" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B188" s="37"/>
+      <c r="C188" s="37"/>
+      <c r="D188" s="37"/>
+      <c r="E188" s="37"/>
+      <c r="F188" s="37"/>
+      <c r="G188" s="8">
+        <f>SUM(G187:G187)</f>
+        <v>0</v>
+      </c>
+      <c r="H188" s="21">
+        <f>SUM(H187:H187)</f>
+        <v>0</v>
+      </c>
+      <c r="I188" s="22">
+        <f>SUM(I187:I187)</f>
+        <v>0</v>
+      </c>
+      <c r="J188" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A189" s="10"/>
+      <c r="D189" s="9"/>
+      <c r="E189" s="9"/>
+      <c r="F189" s="11"/>
+      <c r="G189" s="12"/>
+      <c r="H189" s="11"/>
+      <c r="I189" s="9"/>
+      <c r="J189" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A190" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="B190" s="14"/>
+      <c r="C190" s="14"/>
+      <c r="D190" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="E190" s="14"/>
+      <c r="F190" s="14"/>
+      <c r="G190" s="14"/>
+      <c r="H190" s="14"/>
+      <c r="I190" s="16"/>
+      <c r="J190" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A191" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H191" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I191" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J191" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A192" s="5">
+        <v>1</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D192" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F192" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="G192" s="56" t="s">
+        <v>435</v>
+      </c>
+      <c r="H192" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="I192" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="J192" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A193" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B193" s="37"/>
+      <c r="C193" s="37"/>
+      <c r="D193" s="37"/>
+      <c r="E193" s="37"/>
+      <c r="F193" s="37"/>
+      <c r="G193" s="8">
+        <f>SUM(G192:G192)</f>
+        <v>0</v>
+      </c>
+      <c r="H193" s="24">
+        <f>SUM(H192:H192)</f>
+        <v>0</v>
+      </c>
+      <c r="I193" s="25">
+        <f>SUM(I192:I192)</f>
+        <v>0</v>
+      </c>
+      <c r="J193" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A194" s="10"/>
+      <c r="D194" s="9"/>
+      <c r="E194" s="9"/>
+      <c r="F194" s="11"/>
+      <c r="G194" s="12"/>
+      <c r="H194" s="11"/>
+      <c r="I194" s="9"/>
+      <c r="J194" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A195" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B196" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C196" s="30"/>
+      <c r="D196" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H196" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A197" s="5">
+        <v>1</v>
+      </c>
+      <c r="B197" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C197" s="38"/>
+      <c r="D197" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E197" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F197" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G197" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H197" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I197" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A198" s="34" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B165" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C165" s="26"/>
-      <c r="D165" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G165" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H165" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A166" s="5">
-        <v>1</v>
-      </c>
-      <c r="B166" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="C166" s="37"/>
-      <c r="D166" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="E166" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="F166" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="G166" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="H166" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="I166" s="48" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A167" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="B167" s="31"/>
-      <c r="C167" s="31"/>
-      <c r="D167" s="31"/>
-      <c r="E167" s="31"/>
-      <c r="F167" s="31"/>
-      <c r="G167" s="31"/>
-      <c r="H167" s="32"/>
-      <c r="I167" s="48" t="s">
+      <c r="B198" s="35"/>
+      <c r="C198" s="35"/>
+      <c r="D198" s="35"/>
+      <c r="E198" s="35"/>
+      <c r="F198" s="35"/>
+      <c r="G198" s="35"/>
+      <c r="H198" s="36"/>
+      <c r="I198" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A168" s="20" t="s">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A199" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B168" s="36"/>
-      <c r="C168" s="36"/>
-      <c r="D168" s="36"/>
-      <c r="E168" s="36"/>
-      <c r="F168" s="40">
-        <f>SUM(F166:F166)</f>
-        <v>0</v>
-      </c>
-      <c r="G168" s="40">
-        <f>SUM(G166:G166)</f>
-        <v>0</v>
-      </c>
-      <c r="H168" s="41">
-        <f>SUM(H166:H166)</f>
+      <c r="B199" s="33"/>
+      <c r="C199" s="33"/>
+      <c r="D199" s="33"/>
+      <c r="E199" s="33"/>
+      <c r="F199" s="21">
+        <f>SUM(F197:F197)</f>
+        <v>0</v>
+      </c>
+      <c r="G199" s="21">
+        <f>SUM(G197:G197)</f>
+        <v>0</v>
+      </c>
+      <c r="H199" s="22">
+        <f>SUM(H197:H197)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="A168:E168"/>
-    <mergeCell ref="A167:H167"/>
-    <mergeCell ref="A77:F77"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A97:F97"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A122:F122"/>
-    <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A87:F87"/>
+  <mergeCells count="64">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A57:F57"/>
     <mergeCell ref="A72:F72"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B197:C197"/>
     <mergeCell ref="B145:C145"/>
     <mergeCell ref="B146:C146"/>
     <mergeCell ref="A132:F132"/>
@@ -5945,34 +6822,30 @@
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B153:C153"/>
     <mergeCell ref="B154:C154"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A168:F168"/>
+    <mergeCell ref="A173:F173"/>
+    <mergeCell ref="A178:F178"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A97:F97"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="A199:E199"/>
+    <mergeCell ref="A198:H198"/>
+    <mergeCell ref="A183:F183"/>
+    <mergeCell ref="A188:F188"/>
+    <mergeCell ref="A193:F193"/>
+    <mergeCell ref="A172:I172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: update export_billing_detail.xlsx with new data
</commit_message>
<xml_diff>
--- a/resources/xlsx/export_billing_detail.xlsx
+++ b/resources/xlsx/export_billing_detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mmj\project\PHP\MARGO-BARU\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B2D8E0-D41F-4AEB-9E43-DBEE0B8946E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFB28AB-BFDF-4E80-9025-B60B98C717B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{16F53B30-EA35-46C9-9529-5DBEDB6DC1E5}"/>
   </bookViews>
@@ -2169,8 +2169,8 @@
   </sheetPr>
   <dimension ref="A2:L199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>